<commit_message>
Updated excel file to have header column for apps
</commit_message>
<xml_diff>
--- a/apps_info.xlsx
+++ b/apps_info.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Dropbox\programming\python\scratchpad\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Dropbox\programming\projects\check-app-versions\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CC0976FE-EA85-452B-98C5-BEE8DAAA4487}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B8614663-3F32-402A-A428-61033F3CABE3}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="480" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3480" yWindow="1485" windowWidth="21000" windowHeight="13380" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -799,8 +799,8 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="25.140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="17.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="18.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="25.140625" style="1" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="19.85546875" style="1" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="88.7109375" style="1" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="57.5703125" style="1" bestFit="1" customWidth="1"/>
@@ -809,10 +809,10 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>0</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>71</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>1</v>
@@ -826,10 +826,10 @@
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="B2" s="1" t="s">
         <v>4</v>
-      </c>
-      <c r="B2" s="1" t="s">
-        <v>72</v>
       </c>
       <c r="C2" s="1" t="s">
         <v>5</v>
@@ -843,10 +843,10 @@
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="B3" s="1" t="s">
         <v>8</v>
-      </c>
-      <c r="B3" s="1" t="s">
-        <v>73</v>
       </c>
       <c r="C3" s="1" t="s">
         <v>9</v>
@@ -860,10 +860,10 @@
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="B4" s="1" t="s">
         <v>13</v>
-      </c>
-      <c r="B4" s="1" t="s">
-        <v>74</v>
       </c>
       <c r="C4" s="1" t="s">
         <v>42</v>
@@ -877,10 +877,10 @@
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="B5" s="1" t="s">
         <v>15</v>
-      </c>
-      <c r="B5" s="1" t="s">
-        <v>75</v>
       </c>
       <c r="C5" s="1" t="s">
         <v>43</v>
@@ -911,10 +911,10 @@
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="B7" s="1" t="s">
         <v>17</v>
-      </c>
-      <c r="B7" s="1" t="s">
-        <v>76</v>
       </c>
       <c r="C7" s="1" t="s">
         <v>45</v>
@@ -928,10 +928,10 @@
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="B8" s="1" t="s">
         <v>17</v>
-      </c>
-      <c r="B8" s="1" t="s">
-        <v>92</v>
       </c>
       <c r="C8" s="1" t="s">
         <v>46</v>
@@ -945,10 +945,10 @@
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="B9" s="1" t="s">
         <v>18</v>
-      </c>
-      <c r="B9" s="1" t="s">
-        <v>77</v>
       </c>
       <c r="C9" s="1" t="s">
         <v>47</v>
@@ -962,10 +962,10 @@
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="B10" s="1" t="s">
         <v>19</v>
-      </c>
-      <c r="B10" s="1" t="s">
-        <v>93</v>
       </c>
       <c r="C10" s="1" t="s">
         <v>48</v>
@@ -979,10 +979,10 @@
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="B11" s="1" t="s">
         <v>20</v>
-      </c>
-      <c r="B11" s="1" t="s">
-        <v>94</v>
       </c>
       <c r="C11" s="1" t="s">
         <v>49</v>
@@ -996,10 +996,10 @@
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="B12" s="1" t="s">
         <v>21</v>
-      </c>
-      <c r="B12" s="1" t="s">
-        <v>95</v>
       </c>
       <c r="C12" s="1" t="s">
         <v>50</v>
@@ -1013,10 +1013,10 @@
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="B13" s="1" t="s">
         <v>22</v>
-      </c>
-      <c r="B13" s="1" t="s">
-        <v>78</v>
       </c>
       <c r="C13" s="1" t="s">
         <v>51</v>
@@ -1030,10 +1030,10 @@
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="B14" s="1" t="s">
         <v>23</v>
-      </c>
-      <c r="B14" s="1" t="s">
-        <v>79</v>
       </c>
       <c r="C14" s="1" t="s">
         <v>52</v>
@@ -1047,10 +1047,10 @@
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="B15" s="1" t="s">
         <v>24</v>
-      </c>
-      <c r="B15" s="1" t="s">
-        <v>80</v>
       </c>
       <c r="C15" s="1" t="s">
         <v>53</v>
@@ -1064,10 +1064,10 @@
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="B16" s="1" t="s">
         <v>25</v>
-      </c>
-      <c r="B16" s="1" t="s">
-        <v>81</v>
       </c>
       <c r="C16" s="1" t="s">
         <v>54</v>
@@ -1081,10 +1081,10 @@
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="B17" s="1" t="s">
         <v>26</v>
-      </c>
-      <c r="B17" s="1" t="s">
-        <v>82</v>
       </c>
       <c r="C17" s="1" t="s">
         <v>55</v>
@@ -1098,10 +1098,10 @@
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="B18" s="1" t="s">
         <v>27</v>
-      </c>
-      <c r="B18" s="1" t="s">
-        <v>83</v>
       </c>
       <c r="C18" s="1" t="s">
         <v>56</v>
@@ -1115,10 +1115,10 @@
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="B19" s="1" t="s">
         <v>28</v>
-      </c>
-      <c r="B19" s="1" t="s">
-        <v>84</v>
       </c>
       <c r="C19" s="1" t="s">
         <v>57</v>
@@ -1132,10 +1132,10 @@
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="B20" s="1" t="s">
         <v>29</v>
-      </c>
-      <c r="B20" s="1" t="s">
-        <v>85</v>
       </c>
       <c r="C20" s="1" t="s">
         <v>58</v>
@@ -1149,10 +1149,10 @@
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A21" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="B21" s="1" t="s">
         <v>30</v>
-      </c>
-      <c r="B21" s="1" t="s">
-        <v>86</v>
       </c>
       <c r="C21" s="1" t="s">
         <v>59</v>
@@ -1166,10 +1166,10 @@
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A22" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="B22" s="1" t="s">
         <v>31</v>
-      </c>
-      <c r="B22" s="1" t="s">
-        <v>96</v>
       </c>
       <c r="C22" s="1" t="s">
         <v>60</v>
@@ -1183,10 +1183,10 @@
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A23" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="B23" s="1" t="s">
         <v>32</v>
-      </c>
-      <c r="B23" s="1" t="s">
-        <v>87</v>
       </c>
       <c r="C23" s="1" t="s">
         <v>61</v>
@@ -1200,10 +1200,10 @@
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A24" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="B24" s="1" t="s">
         <v>33</v>
-      </c>
-      <c r="B24" s="1" t="s">
-        <v>88</v>
       </c>
       <c r="C24" s="1" t="s">
         <v>62</v>
@@ -1217,10 +1217,10 @@
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A25" s="1" t="s">
+        <v>97</v>
+      </c>
+      <c r="B25" s="1" t="s">
         <v>34</v>
-      </c>
-      <c r="B25" s="1" t="s">
-        <v>97</v>
       </c>
       <c r="C25" s="1" t="s">
         <v>63</v>
@@ -1234,10 +1234,10 @@
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A26" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="B26" s="1" t="s">
         <v>35</v>
-      </c>
-      <c r="B26" s="1" t="s">
-        <v>98</v>
       </c>
       <c r="C26" s="1" t="s">
         <v>64</v>
@@ -1251,10 +1251,10 @@
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A27" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="B27" s="1" t="s">
         <v>36</v>
-      </c>
-      <c r="B27" s="1" t="s">
-        <v>99</v>
       </c>
       <c r="C27" s="1" t="s">
         <v>65</v>
@@ -1268,10 +1268,10 @@
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A28" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="B28" s="1" t="s">
         <v>37</v>
-      </c>
-      <c r="B28" s="1" t="s">
-        <v>89</v>
       </c>
       <c r="C28" s="1" t="s">
         <v>66</v>
@@ -1285,10 +1285,10 @@
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A29" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="B29" s="1" t="s">
         <v>38</v>
-      </c>
-      <c r="B29" s="1" t="s">
-        <v>90</v>
       </c>
       <c r="C29" s="1" t="s">
         <v>67</v>
@@ -1302,10 +1302,10 @@
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A30" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="B30" s="1" t="s">
         <v>39</v>
-      </c>
-      <c r="B30" s="1" t="s">
-        <v>91</v>
       </c>
       <c r="C30" s="1" t="s">
         <v>68</v>
@@ -1319,10 +1319,10 @@
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A31" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="B31" s="1" t="s">
         <v>40</v>
-      </c>
-      <c r="B31" s="1" t="s">
-        <v>100</v>
       </c>
       <c r="C31" s="1" t="s">
         <v>69</v>
@@ -1336,10 +1336,10 @@
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A32" s="1" t="s">
+        <v>101</v>
+      </c>
+      <c r="B32" s="1" t="s">
         <v>41</v>
-      </c>
-      <c r="B32" s="1" t="s">
-        <v>101</v>
       </c>
       <c r="C32" s="1" t="s">
         <v>70</v>

</xml_diff>

<commit_message>
Modified typo for crystaldiskmark app
</commit_message>
<xml_diff>
--- a/apps_info.xlsx
+++ b/apps_info.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Dropbox\programming\projects\check-app-versions\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B8614663-3F32-402A-A428-61033F3CABE3}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6DC01D79-6F8C-4BA7-8FF4-5F6AEF2E6A7F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="3480" yWindow="1485" windowWidth="21000" windowHeight="13380" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="160" uniqueCount="150">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="160" uniqueCount="151">
   <si>
     <t>app_name</t>
   </si>
@@ -475,6 +475,9 @@
   </si>
   <si>
     <t>//h4[@class="sub"]/text()</t>
+  </si>
+  <si>
+    <t>CrystalDiskMark</t>
   </si>
 </sst>
 </file>
@@ -795,7 +798,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E32"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B9" sqref="B9"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -931,7 +936,7 @@
         <v>92</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>17</v>
+        <v>150</v>
       </c>
       <c r="C8" s="1" t="s">
         <v>46</v>

</xml_diff>

<commit_message>
Fixed mismatched information at the bottom rows
</commit_message>
<xml_diff>
--- a/apps_info.xlsx
+++ b/apps_info.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Dropbox\programming\projects\check-app-versions\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6DC01D79-6F8C-4BA7-8FF4-5F6AEF2E6A7F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7A9A5501-34F7-4280-8B0E-FC502D31378A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3480" yWindow="1485" windowWidth="21000" windowHeight="13380" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2205" yWindow="930" windowWidth="21000" windowHeight="13380" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -42,9 +42,6 @@
     <t>Visual C Redistributable</t>
   </si>
   <si>
-    <t>0.27.0</t>
-  </si>
-  <si>
     <t>https://github.com/abbodi1406/vcredist/releases</t>
   </si>
   <si>
@@ -156,9 +153,6 @@
     <t>2.3.3</t>
   </si>
   <si>
-    <t>4.11.2</t>
-  </si>
-  <si>
     <t>1.3.14</t>
   </si>
   <si>
@@ -168,9 +162,6 @@
     <t>7.0.0g</t>
   </si>
   <si>
-    <t>91.4.548</t>
-  </si>
-  <si>
     <t>1.2.1</t>
   </si>
   <si>
@@ -186,15 +177,6 @@
     <t>7.4</t>
   </si>
   <si>
-    <t>20200223-90913ab</t>
-  </si>
-  <si>
-    <t>73.0.1</t>
-  </si>
-  <si>
-    <t>2.25.1</t>
-  </si>
-  <si>
     <t>1.2.10.6</t>
   </si>
   <si>
@@ -225,15 +207,9 @@
     <t>1.42</t>
   </si>
   <si>
-    <t>5.17</t>
-  </si>
-  <si>
     <t>3.8.1</t>
   </si>
   <si>
-    <t>3.8</t>
-  </si>
-  <si>
     <t>4.7.1</t>
   </si>
   <si>
@@ -478,6 +454,30 @@
   </si>
   <si>
     <t>CrystalDiskMark</t>
+  </si>
+  <si>
+    <t>0.26.0</t>
+  </si>
+  <si>
+    <t>4.9.1</t>
+  </si>
+  <si>
+    <t>89.4.278</t>
+  </si>
+  <si>
+    <t>72.0.2</t>
+  </si>
+  <si>
+    <t>20200131-62d92a8</t>
+  </si>
+  <si>
+    <t>2.25.0</t>
+  </si>
+  <si>
+    <t>1.41.1</t>
+  </si>
+  <si>
+    <t>5.15.9</t>
   </si>
 </sst>
 </file>
@@ -798,9 +798,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E32"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -814,7 +812,7 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>71</v>
+        <v>63</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>0</v>
@@ -831,529 +829,529 @@
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
-        <v>72</v>
+        <v>64</v>
       </c>
       <c r="B2" s="1" t="s">
         <v>4</v>
       </c>
       <c r="C2" s="1" t="s">
+        <v>143</v>
+      </c>
+      <c r="D2" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="D2" s="1" t="s">
+      <c r="E2" s="1" t="s">
         <v>6</v>
-      </c>
-      <c r="E2" s="1" t="s">
-        <v>7</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
-        <v>73</v>
+        <v>65</v>
       </c>
       <c r="B3" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C3" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="C3" s="1" t="s">
+      <c r="D3" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="D3" s="1" t="s">
+      <c r="E3" s="1" t="s">
         <v>10</v>
-      </c>
-      <c r="E3" s="1" t="s">
-        <v>11</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
-        <v>74</v>
+        <v>66</v>
       </c>
       <c r="B4" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E4" s="1" t="s">
         <v>13</v>
-      </c>
-      <c r="C4" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="D4" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="E4" s="1" t="s">
-        <v>14</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
-        <v>75</v>
+        <v>67</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>43</v>
+        <v>144</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>102</v>
+        <v>94</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>103</v>
+        <v>95</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>104</v>
+        <v>96</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
-        <v>76</v>
+        <v>68</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>105</v>
+        <v>97</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>106</v>
+        <v>98</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
-        <v>92</v>
+        <v>84</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>150</v>
+        <v>142</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>105</v>
+        <v>97</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>107</v>
+        <v>99</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
-        <v>77</v>
+        <v>69</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>47</v>
+        <v>145</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>108</v>
+        <v>100</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>109</v>
+        <v>101</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
-        <v>93</v>
+        <v>85</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>110</v>
+        <v>102</v>
       </c>
       <c r="E10" s="1" t="s">
-        <v>111</v>
+        <v>103</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
-        <v>94</v>
+        <v>86</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>113</v>
+        <v>105</v>
       </c>
       <c r="E11" s="1" t="s">
-        <v>114</v>
+        <v>106</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
-        <v>95</v>
+        <v>87</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="D12" s="1" t="s">
-        <v>115</v>
+        <v>107</v>
       </c>
       <c r="E12" s="1" t="s">
-        <v>116</v>
+        <v>108</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
-        <v>78</v>
+        <v>70</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="D13" s="1" t="s">
-        <v>117</v>
+        <v>109</v>
       </c>
       <c r="E13" s="1" t="s">
-        <v>118</v>
+        <v>110</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
-        <v>79</v>
+        <v>71</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="D14" s="1" t="s">
-        <v>119</v>
+        <v>111</v>
       </c>
       <c r="E14" s="1" t="s">
-        <v>120</v>
+        <v>112</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
-        <v>80</v>
+        <v>72</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>53</v>
+        <v>147</v>
       </c>
       <c r="D15" s="1" t="s">
-        <v>121</v>
+        <v>113</v>
       </c>
       <c r="E15" s="1" t="s">
-        <v>122</v>
+        <v>114</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
-        <v>81</v>
+        <v>73</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>54</v>
+        <v>146</v>
       </c>
       <c r="D16" s="1" t="s">
-        <v>112</v>
+        <v>104</v>
       </c>
       <c r="E16" s="1" t="s">
-        <v>109</v>
+        <v>101</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
-        <v>82</v>
+        <v>74</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>55</v>
+        <v>148</v>
       </c>
       <c r="D17" s="1" t="s">
-        <v>123</v>
+        <v>115</v>
       </c>
       <c r="E17" s="1" t="s">
-        <v>124</v>
+        <v>116</v>
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
-        <v>83</v>
+        <v>75</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>56</v>
+        <v>50</v>
       </c>
       <c r="D18" s="1" t="s">
-        <v>125</v>
+        <v>117</v>
       </c>
       <c r="E18" s="1" t="s">
-        <v>126</v>
+        <v>118</v>
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
-        <v>84</v>
+        <v>76</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>57</v>
+        <v>51</v>
       </c>
       <c r="D19" s="1" t="s">
-        <v>127</v>
+        <v>119</v>
       </c>
       <c r="E19" s="1" t="s">
-        <v>128</v>
+        <v>120</v>
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
-        <v>85</v>
+        <v>77</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>58</v>
+        <v>52</v>
       </c>
       <c r="D20" s="1" t="s">
-        <v>129</v>
+        <v>121</v>
       </c>
       <c r="E20" s="1" t="s">
-        <v>130</v>
+        <v>122</v>
       </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A21" s="1" t="s">
-        <v>86</v>
+        <v>78</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>59</v>
+        <v>53</v>
       </c>
       <c r="D21" s="1" t="s">
-        <v>131</v>
+        <v>123</v>
       </c>
       <c r="E21" s="1" t="s">
-        <v>109</v>
+        <v>101</v>
       </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A22" s="1" t="s">
-        <v>96</v>
+        <v>88</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C22" s="1" t="s">
-        <v>60</v>
+        <v>54</v>
       </c>
       <c r="D22" s="1" t="s">
-        <v>132</v>
+        <v>124</v>
       </c>
       <c r="E22" s="1" t="s">
-        <v>133</v>
+        <v>125</v>
       </c>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A23" s="1" t="s">
-        <v>87</v>
+        <v>79</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C23" s="1" t="s">
-        <v>61</v>
+        <v>55</v>
       </c>
       <c r="D23" s="1" t="s">
-        <v>134</v>
+        <v>126</v>
       </c>
       <c r="E23" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A24" s="1" t="s">
-        <v>88</v>
+        <v>80</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C24" s="1" t="s">
-        <v>62</v>
+        <v>56</v>
       </c>
       <c r="D24" s="1" t="s">
-        <v>135</v>
+        <v>127</v>
       </c>
       <c r="E24" s="1" t="s">
-        <v>136</v>
+        <v>128</v>
       </c>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A25" s="1" t="s">
-        <v>97</v>
+        <v>89</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C25" s="1" t="s">
-        <v>63</v>
+        <v>57</v>
       </c>
       <c r="D25" s="1" t="s">
-        <v>137</v>
+        <v>129</v>
       </c>
       <c r="E25" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A26" s="1" t="s">
-        <v>98</v>
+        <v>82</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="C26" s="1" t="s">
-        <v>64</v>
+        <v>60</v>
       </c>
       <c r="D26" s="1" t="s">
-        <v>138</v>
+        <v>130</v>
       </c>
       <c r="E26" s="1" t="s">
-        <v>139</v>
+        <v>131</v>
       </c>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A27" s="1" t="s">
-        <v>99</v>
+        <v>83</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="C27" s="1" t="s">
-        <v>65</v>
+        <v>59</v>
       </c>
       <c r="D27" s="1" t="s">
-        <v>140</v>
-      </c>
-      <c r="E27" s="1" t="s">
-        <v>7</v>
+        <v>132</v>
+      </c>
+      <c r="E27" t="s">
+        <v>6</v>
       </c>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A28" s="1" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="C28" s="1" t="s">
-        <v>66</v>
+        <v>58</v>
       </c>
       <c r="D28" s="1" t="s">
-        <v>141</v>
-      </c>
-      <c r="E28" s="1" t="s">
-        <v>142</v>
+        <v>133</v>
+      </c>
+      <c r="E28" t="s">
+        <v>134</v>
       </c>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A29" s="1" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="C29" s="1" t="s">
-        <v>67</v>
+        <v>149</v>
       </c>
       <c r="D29" s="1" t="s">
-        <v>143</v>
-      </c>
-      <c r="E29" s="1" t="s">
-        <v>144</v>
+        <v>135</v>
+      </c>
+      <c r="E29" t="s">
+        <v>136</v>
       </c>
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A30" s="1" t="s">
-        <v>91</v>
+        <v>81</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="C30" s="1" t="s">
-        <v>68</v>
+        <v>150</v>
       </c>
       <c r="D30" s="1" t="s">
-        <v>145</v>
-      </c>
-      <c r="E30" s="1" t="s">
-        <v>146</v>
+        <v>137</v>
+      </c>
+      <c r="E30" t="s">
+        <v>138</v>
       </c>
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A31" s="1" t="s">
-        <v>100</v>
+        <v>92</v>
       </c>
       <c r="B31" s="1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C31" s="1" t="s">
-        <v>69</v>
+        <v>61</v>
       </c>
       <c r="D31" s="1" t="s">
-        <v>147</v>
-      </c>
-      <c r="E31" s="1" t="s">
-        <v>7</v>
+        <v>139</v>
+      </c>
+      <c r="E31" t="s">
+        <v>6</v>
       </c>
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A32" s="1" t="s">
-        <v>101</v>
+        <v>93</v>
       </c>
       <c r="B32" s="1" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C32" s="1" t="s">
-        <v>70</v>
+        <v>62</v>
       </c>
       <c r="D32" s="1" t="s">
-        <v>148</v>
+        <v>140</v>
       </c>
       <c r="E32" s="1" t="s">
-        <v>149</v>
+        <v>141</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updated apps list and versions
</commit_message>
<xml_diff>
--- a/apps_info.xlsx
+++ b/apps_info.xlsx
@@ -514,7 +514,7 @@
       </c>
       <c r="C7" s="1" t="inlineStr">
         <is>
-          <t>8.4.1</t>
+          <t>8.4.2</t>
         </is>
       </c>
       <c r="D7" s="1" t="inlineStr">
@@ -622,7 +622,7 @@
       </c>
       <c r="C11" s="1" t="inlineStr">
         <is>
-          <t>2019-10-14</t>
+          <t>2020-03-08</t>
         </is>
       </c>
       <c r="D11" s="1" t="inlineStr">
@@ -703,7 +703,7 @@
       </c>
       <c r="C14" s="1" t="inlineStr">
         <is>
-          <t>7.4</t>
+          <t>7.5</t>
         </is>
       </c>
       <c r="D14" s="1" t="inlineStr">
@@ -730,7 +730,7 @@
       </c>
       <c r="C15" s="1" t="inlineStr">
         <is>
-          <t>20200303-60b1f85</t>
+          <t>20200312-675bb1f</t>
         </is>
       </c>
       <c r="D15" s="1" t="inlineStr">
@@ -757,7 +757,7 @@
       </c>
       <c r="C16" s="1" t="inlineStr">
         <is>
-          <t>73.0.1</t>
+          <t>74.0</t>
         </is>
       </c>
       <c r="D16" s="1" t="inlineStr">
@@ -946,7 +946,7 @@
       </c>
       <c r="C23" s="1" t="inlineStr">
         <is>
-          <t>43.0.0</t>
+          <t>44.0.0</t>
         </is>
       </c>
       <c r="D23" s="1" t="inlineStr">
@@ -1108,7 +1108,7 @@
       </c>
       <c r="C29" s="1" t="inlineStr">
         <is>
-          <t>1.42</t>
+          <t>1.43</t>
         </is>
       </c>
       <c r="D29" s="1" t="inlineStr">
@@ -1135,7 +1135,7 @@
       </c>
       <c r="C30" s="1" t="inlineStr">
         <is>
-          <t>5.17.1</t>
+          <t>5.17.2</t>
         </is>
       </c>
       <c r="D30" s="1" t="inlineStr">

</xml_diff>

<commit_message>
Updated excel file with latest info
</commit_message>
<xml_diff>
--- a/apps_info.xlsx
+++ b/apps_info.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <bookViews>
-    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="-120" yWindow="480" windowWidth="29040" windowHeight="15840" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
+    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="3780" yWindow="1740" windowWidth="21000" windowHeight="13380" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
     <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
@@ -323,7 +323,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F32"/>
+  <dimension ref="A1:F31"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -337,8 +337,8 @@
     <col width="47.140625" customWidth="1" style="1" min="4" max="4"/>
     <col width="88.7109375" bestFit="1" customWidth="1" style="1" min="5" max="5"/>
     <col width="55.85546875" customWidth="1" style="1" min="6" max="6"/>
-    <col width="9.140625" customWidth="1" style="1" min="7" max="10"/>
-    <col width="9.140625" customWidth="1" style="1" min="11" max="16384"/>
+    <col width="9.140625" customWidth="1" style="1" min="7" max="13"/>
+    <col width="9.140625" customWidth="1" style="1" min="14" max="16384"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -386,7 +386,7 @@
       </c>
       <c r="C2" s="1" t="inlineStr">
         <is>
-          <t>0.29.0</t>
+          <t>0.30.0</t>
         </is>
       </c>
       <c r="D2" s="1" t="inlineStr">
@@ -450,7 +450,7 @@
       </c>
       <c r="C4" s="1" t="inlineStr">
         <is>
-          <t>2.3.3</t>
+          <t>2.4.1</t>
         </is>
       </c>
       <c r="D4" s="1" t="inlineStr">
@@ -482,7 +482,7 @@
       </c>
       <c r="C5" s="1" t="inlineStr">
         <is>
-          <t>4.14.0</t>
+          <t>4.16.0</t>
         </is>
       </c>
       <c r="D5" s="1" t="inlineStr">
@@ -546,7 +546,7 @@
       </c>
       <c r="C7" s="1" t="inlineStr">
         <is>
-          <t>8.4.2</t>
+          <t>8.5.2</t>
         </is>
       </c>
       <c r="D7" s="1" t="inlineStr">
@@ -610,7 +610,7 @@
       </c>
       <c r="C9" s="1" t="inlineStr">
         <is>
-          <t>95.4.441</t>
+          <t>97.4.467</t>
         </is>
       </c>
       <c r="D9" s="1" t="inlineStr">
@@ -738,7 +738,7 @@
       </c>
       <c r="C13" s="1" t="inlineStr">
         <is>
-          <t>11.96</t>
+          <t>11.99</t>
         </is>
       </c>
       <c r="D13" s="1" t="inlineStr">
@@ -792,574 +792,542 @@
     <row r="15">
       <c r="A15" s="1" t="inlineStr">
         <is>
-          <t>ffmpeg</t>
+          <t>firefox</t>
         </is>
       </c>
       <c r="B15" s="1" t="inlineStr">
         <is>
-          <t>FFmpeg</t>
+          <t>Firefox</t>
         </is>
       </c>
       <c r="C15" s="1" t="inlineStr">
         <is>
-          <t>20200424-a501947</t>
+          <t>76.0.1</t>
         </is>
       </c>
       <c r="D15" s="1" t="inlineStr">
         <is>
-          <t>https://ffmpeg.zeranoe.com/builds</t>
+          <t>https://en.wikipedia.org/wiki/Firefox</t>
         </is>
       </c>
       <c r="E15" s="1" t="inlineStr">
         <is>
-          <t>https://ffmpeg.zeranoe.com/builds</t>
+          <t>https://download.mozilla.org/?product=firefox-latest-ssl^&amp;os=win64^&amp;lang=en-US</t>
         </is>
       </c>
       <c r="F15" s="1" t="inlineStr">
         <is>
-          <t>//label[@class="btn btn-secondary active"]/text()</t>
+          <t>//table[@class="infobox vevent"]/tbody/tr/td//text()</t>
         </is>
       </c>
     </row>
     <row r="16">
       <c r="A16" s="1" t="inlineStr">
         <is>
-          <t>firefox</t>
+          <t>git</t>
         </is>
       </c>
       <c r="B16" s="1" t="inlineStr">
         <is>
-          <t>Firefox</t>
+          <t>Git</t>
         </is>
       </c>
       <c r="C16" s="1" t="inlineStr">
         <is>
-          <t>75.0</t>
+          <t>2.26.2</t>
         </is>
       </c>
       <c r="D16" s="1" t="inlineStr">
         <is>
-          <t>https://en.wikipedia.org/wiki/Firefox</t>
+          <t>https://git-scm.com/download/win</t>
         </is>
       </c>
       <c r="E16" s="1" t="inlineStr">
         <is>
-          <t>https://download.mozilla.org/?product=firefox-latest-ssl^&amp;os=win64^&amp;lang=en-US</t>
+          <t>https://git-scm.com/download/win</t>
         </is>
       </c>
       <c r="F16" s="1" t="inlineStr">
         <is>
-          <t>//table[@class="infobox vevent"]/tbody/tr/td//text()</t>
+          <t>//p[1]/strong[1]/text()</t>
         </is>
       </c>
     </row>
     <row r="17">
       <c r="A17" s="1" t="inlineStr">
         <is>
-          <t>git</t>
+          <t>greenshot</t>
         </is>
       </c>
       <c r="B17" s="1" t="inlineStr">
         <is>
-          <t>Git</t>
+          <t>Greenshot</t>
         </is>
       </c>
       <c r="C17" s="1" t="inlineStr">
         <is>
-          <t>2.26.2</t>
+          <t>1.2.10.6</t>
         </is>
       </c>
       <c r="D17" s="1" t="inlineStr">
         <is>
-          <t>https://git-scm.com/download/win</t>
+          <t>https://getgreenshot.org/downloads</t>
         </is>
       </c>
       <c r="E17" s="1" t="inlineStr">
         <is>
-          <t>https://git-scm.com/download/win</t>
+          <t>https://getgreenshot.org/downloads</t>
         </is>
       </c>
       <c r="F17" s="1" t="inlineStr">
         <is>
-          <t>//p[1]/strong[1]/text()</t>
+          <t>//div[2]/div[1]/div[1]/text()</t>
         </is>
       </c>
     </row>
     <row r="18">
       <c r="A18" s="1" t="inlineStr">
         <is>
-          <t>greenshot</t>
+          <t>hashtab</t>
         </is>
       </c>
       <c r="B18" s="1" t="inlineStr">
         <is>
-          <t>Greenshot</t>
+          <t>Hashtab</t>
         </is>
       </c>
       <c r="C18" s="1" t="inlineStr">
         <is>
-          <t>1.2.10.6</t>
+          <t>6.0.0.34</t>
         </is>
       </c>
       <c r="D18" s="1" t="inlineStr">
         <is>
-          <t>https://getgreenshot.org/downloads</t>
+          <t>http://implbits.com/products/hashtab</t>
         </is>
       </c>
       <c r="E18" s="1" t="inlineStr">
         <is>
-          <t>https://getgreenshot.org/downloads</t>
+          <t>http://implbits.com/products/hashtab</t>
         </is>
       </c>
       <c r="F18" s="1" t="inlineStr">
         <is>
-          <t>//div[2]/div[1]/div[1]/text()</t>
+          <t>//a[@id="btn_download_now"]</t>
         </is>
       </c>
     </row>
     <row r="19">
       <c r="A19" s="1" t="inlineStr">
         <is>
-          <t>hashtab</t>
+          <t>hwinfo</t>
         </is>
       </c>
       <c r="B19" s="1" t="inlineStr">
         <is>
-          <t>Hashtab</t>
+          <t>HWInfo</t>
         </is>
       </c>
       <c r="C19" s="1" t="inlineStr">
         <is>
-          <t>6.0.0.34</t>
+          <t>6.26</t>
         </is>
       </c>
       <c r="D19" s="1" t="inlineStr">
         <is>
-          <t>http://implbits.com/products/hashtab</t>
+          <t>https://www.hwinfo.com/download</t>
         </is>
       </c>
       <c r="E19" s="1" t="inlineStr">
         <is>
-          <t>http://implbits.com/products/hashtab</t>
+          <t>https://www.hwinfo.com/download</t>
         </is>
       </c>
       <c r="F19" s="1" t="inlineStr">
         <is>
-          <t>//a[@id="btn_download_now"]</t>
+          <t>//sub/text()</t>
         </is>
       </c>
     </row>
     <row r="20">
       <c r="A20" s="1" t="inlineStr">
         <is>
-          <t>hwinfo</t>
+          <t>itunes</t>
         </is>
       </c>
       <c r="B20" s="1" t="inlineStr">
         <is>
-          <t>HWInfo</t>
+          <t>iTunes</t>
         </is>
       </c>
       <c r="C20" s="1" t="inlineStr">
         <is>
-          <t>6.24</t>
+          <t>12.10.6.2</t>
         </is>
       </c>
       <c r="D20" s="1" t="inlineStr">
         <is>
-          <t>https://www.hwinfo.com/download</t>
+          <t>https://en.wikipedia.org/wiki/ITunes</t>
         </is>
       </c>
       <c r="E20" s="1" t="inlineStr">
         <is>
-          <t>https://www.hwinfo.com/download</t>
+          <t>https://www.apple.com/itunes/download/win64</t>
         </is>
       </c>
       <c r="F20" s="1" t="inlineStr">
         <is>
-          <t>//sub/text()</t>
+          <t>//table[@class="infobox vevent"]/tbody/tr/td//text()</t>
         </is>
       </c>
     </row>
     <row r="21">
       <c r="A21" s="1" t="inlineStr">
         <is>
-          <t>itunes</t>
+          <t>klite_codec</t>
         </is>
       </c>
       <c r="B21" s="1" t="inlineStr">
         <is>
-          <t>iTunes</t>
+          <t>K-Lite Codec</t>
         </is>
       </c>
       <c r="C21" s="1" t="inlineStr">
         <is>
-          <t>12.10.5</t>
+          <t>15.4.8</t>
         </is>
       </c>
       <c r="D21" s="1" t="inlineStr">
         <is>
-          <t>https://en.wikipedia.org/wiki/ITunes</t>
+          <t>https://codecguide.com/download_k-lite_codec_pack_standard.htm</t>
         </is>
       </c>
       <c r="E21" s="1" t="inlineStr">
         <is>
-          <t>https://www.apple.com/itunes/download/win64</t>
+          <t>https://codecguide.com/download_k-lite_codec_pack_standard.htm</t>
         </is>
       </c>
       <c r="F21" s="1" t="inlineStr">
         <is>
-          <t>//table[@class="infobox vevent"]/tbody/tr/td//text()</t>
+          <t>//h4/text()</t>
         </is>
       </c>
     </row>
     <row r="22">
       <c r="A22" s="1" t="inlineStr">
         <is>
-          <t>klite_codec</t>
+          <t>mkvtoolnix</t>
         </is>
       </c>
       <c r="B22" s="1" t="inlineStr">
         <is>
-          <t>K-Lite Codec</t>
+          <t>MKVToolnix</t>
         </is>
       </c>
       <c r="C22" s="1" t="inlineStr">
         <is>
-          <t>15.4.4</t>
+          <t>46.0.0</t>
         </is>
       </c>
       <c r="D22" s="1" t="inlineStr">
         <is>
-          <t>https://codecguide.com/download_k-lite_codec_pack_standard.htm</t>
+          <t>https://www.fosshub.com/MKVToolNix.html</t>
         </is>
       </c>
       <c r="E22" s="1" t="inlineStr">
         <is>
-          <t>https://codecguide.com/download_k-lite_codec_pack_standard.htm</t>
+          <t>https://www.fosshub.com/MKVToolNix.html</t>
         </is>
       </c>
       <c r="F22" s="1" t="inlineStr">
         <is>
-          <t>//h4/text()</t>
+          <t>//dd[@itemprop="softwareVersion"]/text()</t>
         </is>
       </c>
     </row>
     <row r="23">
       <c r="A23" s="1" t="inlineStr">
         <is>
-          <t>mkvtoolnix</t>
+          <t>obs</t>
         </is>
       </c>
       <c r="B23" s="1" t="inlineStr">
         <is>
-          <t>MKVToolnix</t>
+          <t>OBS</t>
         </is>
       </c>
       <c r="C23" s="1" t="inlineStr">
         <is>
-          <t>45.0.0</t>
+          <t>25.0.8</t>
         </is>
       </c>
       <c r="D23" s="1" t="inlineStr">
         <is>
-          <t>https://www.fosshub.com/MKVToolNix.html</t>
+          <t>https://obsproject.com/download</t>
         </is>
       </c>
       <c r="E23" s="1" t="inlineStr">
         <is>
-          <t>https://www.fosshub.com/MKVToolNix.html</t>
+          <t>https://obsproject.com/download</t>
         </is>
       </c>
       <c r="F23" s="1" t="inlineStr">
         <is>
-          <t>//dd[@itemprop="softwareVersion"]/text()</t>
+          <t>//span[@class="dl_ver"]/text()</t>
         </is>
       </c>
     </row>
     <row r="24">
       <c r="A24" s="1" t="inlineStr">
         <is>
-          <t>obs</t>
+          <t>open_shell</t>
         </is>
       </c>
       <c r="B24" s="1" t="inlineStr">
         <is>
-          <t>OBS</t>
+          <t>Open Shell</t>
         </is>
       </c>
       <c r="C24" s="1" t="inlineStr">
         <is>
-          <t>25.0.4</t>
+          <t>4.4.142</t>
         </is>
       </c>
       <c r="D24" s="1" t="inlineStr">
         <is>
-          <t>https://obsproject.com/download</t>
+          <t>https://github.com/Open-Shell/Open-Shell-Menu/releases</t>
         </is>
       </c>
       <c r="E24" s="1" t="inlineStr">
         <is>
-          <t>https://obsproject.com/download</t>
+          <t>https://github.com/Open-Shell/Open-Shell-Menu/releases</t>
         </is>
       </c>
       <c r="F24" s="1" t="inlineStr">
         <is>
-          <t>//span[@class="dl_ver"]/text()</t>
+          <t>//div[@class="f1 flex-auto min-width-0 text-normal"]/a/text()</t>
         </is>
       </c>
     </row>
     <row r="25">
       <c r="A25" s="1" t="inlineStr">
         <is>
-          <t>open_shell</t>
+          <t>python</t>
         </is>
       </c>
       <c r="B25" s="1" t="inlineStr">
         <is>
-          <t>Open Shell</t>
+          <t>Python</t>
         </is>
       </c>
       <c r="C25" s="1" t="inlineStr">
         <is>
-          <t>4.4.142</t>
+          <t>3.8.3</t>
         </is>
       </c>
       <c r="D25" s="1" t="inlineStr">
         <is>
-          <t>https://github.com/Open-Shell/Open-Shell-Menu/releases</t>
+          <t>https://www.python.org/downloads</t>
         </is>
       </c>
       <c r="E25" s="1" t="inlineStr">
         <is>
-          <t>https://github.com/Open-Shell/Open-Shell-Menu/releases</t>
+          <t>https://www.python.org/downloads</t>
         </is>
       </c>
       <c r="F25" s="1" t="inlineStr">
         <is>
-          <t>//div[@class="f1 flex-auto min-width-0 text-normal"]/a/text()</t>
+          <t>//a[@class="button"]/text()</t>
         </is>
       </c>
     </row>
     <row r="26">
       <c r="A26" s="1" t="inlineStr">
         <is>
-          <t>python</t>
+          <t>rufus</t>
         </is>
       </c>
       <c r="B26" s="1" t="inlineStr">
         <is>
-          <t>Python</t>
+          <t>Rufus</t>
         </is>
       </c>
       <c r="C26" s="1" t="inlineStr">
         <is>
-          <t>3.8.2</t>
+          <t>3.10</t>
         </is>
       </c>
       <c r="D26" s="1" t="inlineStr">
         <is>
-          <t>https://www.python.org/downloads</t>
+          <t>https://github.com/pbatard/rufus/releases/latest</t>
         </is>
       </c>
       <c r="E26" s="1" t="inlineStr">
         <is>
-          <t>https://www.python.org/downloads</t>
-        </is>
-      </c>
-      <c r="F26" s="1" t="inlineStr">
-        <is>
-          <t>//a[@class="button"]/text()</t>
+          <t>https://github.com/pbatard/rufus/releases/latest</t>
+        </is>
+      </c>
+      <c r="F26" t="inlineStr">
+        <is>
+          <t>//div[@class="f1 flex-auto min-width-0 text-normal"]/a/text()</t>
         </is>
       </c>
     </row>
     <row r="27">
       <c r="A27" s="1" t="inlineStr">
         <is>
-          <t>rufus</t>
+          <t>sublime_text</t>
         </is>
       </c>
       <c r="B27" s="1" t="inlineStr">
         <is>
-          <t>Rufus</t>
+          <t>Sublime Text</t>
         </is>
       </c>
       <c r="C27" s="1" t="inlineStr">
         <is>
-          <t>3.10</t>
+          <t>3210</t>
         </is>
       </c>
       <c r="D27" s="1" t="inlineStr">
         <is>
-          <t>https://github.com/pbatard/rufus/releases/latest</t>
+          <t>https://www.sublimetext.com/3dev</t>
         </is>
       </c>
       <c r="E27" s="1" t="inlineStr">
         <is>
-          <t>https://github.com/pbatard/rufus/releases/latest</t>
+          <t>https://www.sublimetext.com/3dev</t>
         </is>
       </c>
       <c r="F27" t="inlineStr">
         <is>
-          <t>//div[@class="f1 flex-auto min-width-0 text-normal"]/a/text()</t>
+          <t>//p[@class="latest"]/text()</t>
         </is>
       </c>
     </row>
     <row r="28">
       <c r="A28" s="1" t="inlineStr">
         <is>
-          <t>sublime_text</t>
+          <t>visual_studio_code</t>
         </is>
       </c>
       <c r="B28" s="1" t="inlineStr">
         <is>
-          <t>Sublime Text</t>
+          <t>Visual Studio Code</t>
         </is>
       </c>
       <c r="C28" s="1" t="inlineStr">
         <is>
-          <t>3210</t>
+          <t>1.45</t>
         </is>
       </c>
       <c r="D28" s="1" t="inlineStr">
         <is>
-          <t>https://www.sublimetext.com/3dev</t>
+          <t>https://code.visualstudio.com/updates</t>
         </is>
       </c>
       <c r="E28" s="1" t="inlineStr">
         <is>
-          <t>https://www.sublimetext.com/3dev</t>
+          <t>https://code.visualstudio.com/updates</t>
         </is>
       </c>
       <c r="F28" t="inlineStr">
         <is>
-          <t>//p[@class="latest"]/text()</t>
+          <t>//div[@class="col-sm-9 col-md-8 body"]/h1/text()</t>
         </is>
       </c>
     </row>
     <row r="29">
       <c r="A29" s="1" t="inlineStr">
         <is>
-          <t>visual_studio_code</t>
+          <t>winscp</t>
         </is>
       </c>
       <c r="B29" s="1" t="inlineStr">
         <is>
-          <t>Visual Studio Code</t>
+          <t>WinSCP</t>
         </is>
       </c>
       <c r="C29" s="1" t="inlineStr">
         <is>
-          <t>1.44</t>
+          <t>5.17.5</t>
         </is>
       </c>
       <c r="D29" s="1" t="inlineStr">
         <is>
-          <t>https://code.visualstudio.com/updates</t>
+          <t>https://winscp.net/eng/download.php</t>
         </is>
       </c>
       <c r="E29" s="1" t="inlineStr">
         <is>
-          <t>https://code.visualstudio.com/updates</t>
+          <t>https://winscp.net/eng/download.php</t>
         </is>
       </c>
       <c r="F29" t="inlineStr">
         <is>
-          <t>//div[@class="col-sm-9 col-md-8 body"]/h1/text()</t>
+          <t>//a[@class="btn btn-primary btn-lg"]/text()</t>
         </is>
       </c>
     </row>
     <row r="30">
       <c r="A30" s="1" t="inlineStr">
         <is>
-          <t>winscp</t>
+          <t>g_play_music</t>
         </is>
       </c>
       <c r="B30" s="1" t="inlineStr">
         <is>
-          <t>WinSCP</t>
+          <t>Google Play Music Desktop</t>
         </is>
       </c>
       <c r="C30" s="1" t="inlineStr">
         <is>
-          <t>5.17.4</t>
+          <t>4.7.1</t>
         </is>
       </c>
       <c r="D30" s="1" t="inlineStr">
         <is>
-          <t>https://winscp.net/eng/download.php</t>
+          <t>https://github.com/MarshallOfSound/Google-Play-Music-Desktop-Player-UNOFFICIAL-/releases</t>
         </is>
       </c>
       <c r="E30" s="1" t="inlineStr">
         <is>
-          <t>https://winscp.net/eng/download.php</t>
+          <t>https://github.com/MarshallOfSound/Google-Play-Music-Desktop-Player-UNOFFICIAL-/releases</t>
         </is>
       </c>
       <c r="F30" t="inlineStr">
         <is>
-          <t>//a[@class="btn btn-primary btn-lg"]/text()</t>
+          <t>//div[@class="f1 flex-auto min-width-0 text-normal"]/a/text()</t>
         </is>
       </c>
     </row>
     <row r="31">
       <c r="A31" s="1" t="inlineStr">
         <is>
-          <t>g_play_music</t>
+          <t>java</t>
         </is>
       </c>
       <c r="B31" s="1" t="inlineStr">
         <is>
-          <t>Google Play Music Desktop</t>
+          <t>Java SE</t>
         </is>
       </c>
       <c r="C31" s="1" t="inlineStr">
         <is>
-          <t>4.7.1</t>
+          <t>14.0.1</t>
         </is>
       </c>
       <c r="D31" s="1" t="inlineStr">
         <is>
-          <t>https://github.com/MarshallOfSound/Google-Play-Music-Desktop-Player-UNOFFICIAL-/releases</t>
+          <t>https://www.oracle.com/java/technologies/javase-downloads.html</t>
         </is>
       </c>
       <c r="E31" s="1" t="inlineStr">
         <is>
-          <t>https://github.com/MarshallOfSound/Google-Play-Music-Desktop-Player-UNOFFICIAL-/releases</t>
-        </is>
-      </c>
-      <c r="F31" t="inlineStr">
-        <is>
-          <t>//div[@class="f1 flex-auto min-width-0 text-normal"]/a/text()</t>
-        </is>
-      </c>
-    </row>
-    <row r="32">
-      <c r="A32" s="1" t="inlineStr">
-        <is>
-          <t>java</t>
-        </is>
-      </c>
-      <c r="B32" s="1" t="inlineStr">
-        <is>
-          <t>Java SE</t>
-        </is>
-      </c>
-      <c r="C32" s="1" t="inlineStr">
-        <is>
-          <t>14.0.1</t>
-        </is>
-      </c>
-      <c r="D32" s="1" t="inlineStr">
-        <is>
           <t>https://www.oracle.com/java/technologies/javase-downloads.html</t>
         </is>
       </c>
-      <c r="E32" s="1" t="inlineStr">
-        <is>
-          <t>https://www.oracle.com/java/technologies/javase-downloads.html</t>
-        </is>
-      </c>
-      <c r="F32" s="1" t="inlineStr">
+      <c r="F31" s="1" t="inlineStr">
         <is>
           <t>//p/text()</t>
         </is>

</xml_diff>

<commit_message>
Updated list to reflect latest apps versions from web
</commit_message>
<xml_diff>
--- a/apps_info.xlsx
+++ b/apps_info.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <bookViews>
-    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="3780" yWindow="1740" windowWidth="21000" windowHeight="13380" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
+    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="3030" yWindow="1215" windowWidth="21495" windowHeight="14310" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
     <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
@@ -326,7 +326,7 @@
   <dimension ref="A1:F31"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
+      <selection activeCell="D31" sqref="D31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
@@ -337,8 +337,8 @@
     <col width="47.140625" customWidth="1" style="1" min="4" max="4"/>
     <col width="88.7109375" bestFit="1" customWidth="1" style="1" min="5" max="5"/>
     <col width="55.85546875" customWidth="1" style="1" min="6" max="6"/>
-    <col width="9.140625" customWidth="1" style="1" min="7" max="13"/>
-    <col width="9.140625" customWidth="1" style="1" min="14" max="16384"/>
+    <col width="9.140625" customWidth="1" style="1" min="7" max="14"/>
+    <col width="9.140625" customWidth="1" style="1" min="15" max="16384"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -386,7 +386,7 @@
       </c>
       <c r="C2" s="1" t="inlineStr">
         <is>
-          <t>0.30.0</t>
+          <t>0.31.0</t>
         </is>
       </c>
       <c r="D2" s="1" t="inlineStr">
@@ -482,7 +482,7 @@
       </c>
       <c r="C5" s="1" t="inlineStr">
         <is>
-          <t>4.16.0</t>
+          <t>4.19.0</t>
         </is>
       </c>
       <c r="D5" s="1" t="inlineStr">
@@ -546,7 +546,7 @@
       </c>
       <c r="C7" s="1" t="inlineStr">
         <is>
-          <t>8.5.2</t>
+          <t>8.6.1</t>
         </is>
       </c>
       <c r="D7" s="1" t="inlineStr">
@@ -610,7 +610,7 @@
       </c>
       <c r="C9" s="1" t="inlineStr">
         <is>
-          <t>97.4.467</t>
+          <t>99.4.501</t>
         </is>
       </c>
       <c r="D9" s="1" t="inlineStr">
@@ -738,7 +738,7 @@
       </c>
       <c r="C13" s="1" t="inlineStr">
         <is>
-          <t>11.99</t>
+          <t>12.00</t>
         </is>
       </c>
       <c r="D13" s="1" t="inlineStr">
@@ -802,7 +802,7 @@
       </c>
       <c r="C15" s="1" t="inlineStr">
         <is>
-          <t>76.0.1</t>
+          <t>77.0.1</t>
         </is>
       </c>
       <c r="D15" s="1" t="inlineStr">
@@ -834,7 +834,7 @@
       </c>
       <c r="C16" s="1" t="inlineStr">
         <is>
-          <t>2.26.2</t>
+          <t>2.27.0</t>
         </is>
       </c>
       <c r="D16" s="1" t="inlineStr">
@@ -962,7 +962,7 @@
       </c>
       <c r="C20" s="1" t="inlineStr">
         <is>
-          <t>12.10.6.2</t>
+          <t>12.10.7</t>
         </is>
       </c>
       <c r="D20" s="1" t="inlineStr">
@@ -994,7 +994,7 @@
       </c>
       <c r="C21" s="1" t="inlineStr">
         <is>
-          <t>15.4.8</t>
+          <t>15.5.0</t>
         </is>
       </c>
       <c r="D21" s="1" t="inlineStr">
@@ -1026,7 +1026,7 @@
       </c>
       <c r="C22" s="1" t="inlineStr">
         <is>
-          <t>46.0.0</t>
+          <t>47.0.0</t>
         </is>
       </c>
       <c r="D22" s="1" t="inlineStr">
@@ -1154,7 +1154,7 @@
       </c>
       <c r="C26" s="1" t="inlineStr">
         <is>
-          <t>3.10</t>
+          <t>3.11</t>
         </is>
       </c>
       <c r="D26" s="1" t="inlineStr">
@@ -1218,7 +1218,7 @@
       </c>
       <c r="C28" s="1" t="inlineStr">
         <is>
-          <t>1.45</t>
+          <t>1.46</t>
         </is>
       </c>
       <c r="D28" s="1" t="inlineStr">
@@ -1250,7 +1250,7 @@
       </c>
       <c r="C29" s="1" t="inlineStr">
         <is>
-          <t>5.17.5</t>
+          <t>5.17.6</t>
         </is>
       </c>
       <c r="D29" s="1" t="inlineStr">

</xml_diff>

<commit_message>
Latest excel file with latest apps versions
</commit_message>
<xml_diff>
--- a/apps_info.xlsx
+++ b/apps_info.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <bookViews>
-    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="3030" yWindow="1215" windowWidth="21495" windowHeight="14310" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
+    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="2985" yWindow="3180" windowWidth="21645" windowHeight="12525" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
     <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
@@ -53,6 +53,74 @@
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <colors>
+    <indexedColors>
+      <rgbColor rgb="00000000"/>
+      <rgbColor rgb="00FFFFFF"/>
+      <rgbColor rgb="00FF0000"/>
+      <rgbColor rgb="0000FF00"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00000000"/>
+      <rgbColor rgb="00FFFFFF"/>
+      <rgbColor rgb="00FF0000"/>
+      <rgbColor rgb="0000FF00"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008000"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00808000"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="00C0C0C0"/>
+      <rgbColor rgb="00808080"/>
+      <rgbColor rgb="009999FF"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00FFFFCC"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00660066"/>
+      <rgbColor rgb="00FF8080"/>
+      <rgbColor rgb="000066CC"/>
+      <rgbColor rgb="00CCCCFF"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="0000CCFF"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00CCFFCC"/>
+      <rgbColor rgb="00FFFF99"/>
+      <rgbColor rgb="0099CCFF"/>
+      <rgbColor rgb="00FF99CC"/>
+      <rgbColor rgb="00CC99FF"/>
+      <rgbColor rgb="00FFCC99"/>
+      <rgbColor rgb="003366FF"/>
+      <rgbColor rgb="0033CCCC"/>
+      <rgbColor rgb="0099CC00"/>
+      <rgbColor rgb="00FFCC00"/>
+      <rgbColor rgb="00FF9900"/>
+      <rgbColor rgb="00FF6600"/>
+      <rgbColor rgb="00666699"/>
+      <rgbColor rgb="00969696"/>
+      <rgbColor rgb="00003366"/>
+      <rgbColor rgb="00339966"/>
+      <rgbColor rgb="00003300"/>
+      <rgbColor rgb="00333300"/>
+      <rgbColor rgb="00993300"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00333399"/>
+      <rgbColor rgb="00333333"/>
+    </indexedColors>
+  </colors>
 </styleSheet>
 </file>
 
@@ -326,7 +394,7 @@
   <dimension ref="A1:F31"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D31" sqref="D31"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
@@ -337,8 +405,8 @@
     <col width="47.140625" customWidth="1" style="1" min="4" max="4"/>
     <col width="88.7109375" bestFit="1" customWidth="1" style="1" min="5" max="5"/>
     <col width="55.85546875" customWidth="1" style="1" min="6" max="6"/>
-    <col width="9.140625" customWidth="1" style="1" min="7" max="14"/>
-    <col width="9.140625" customWidth="1" style="1" min="15" max="16384"/>
+    <col width="9.140625" customWidth="1" style="1" min="7" max="15"/>
+    <col width="9.140625" customWidth="1" style="1" min="16" max="16384"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -386,7 +454,7 @@
       </c>
       <c r="C2" s="1" t="inlineStr">
         <is>
-          <t>0.31.0</t>
+          <t>0.33.0</t>
         </is>
       </c>
       <c r="D2" s="1" t="inlineStr">
@@ -450,7 +518,7 @@
       </c>
       <c r="C4" s="1" t="inlineStr">
         <is>
-          <t>2.4.1</t>
+          <t>2.4.2</t>
         </is>
       </c>
       <c r="D4" s="1" t="inlineStr">
@@ -482,7 +550,7 @@
       </c>
       <c r="C5" s="1" t="inlineStr">
         <is>
-          <t>4.19.0</t>
+          <t>4.20.0</t>
         </is>
       </c>
       <c r="D5" s="1" t="inlineStr">
@@ -514,7 +582,7 @@
       </c>
       <c r="C6" s="1" t="inlineStr">
         <is>
-          <t>1.3.14</t>
+          <t>1.3.15 2020/06/26</t>
         </is>
       </c>
       <c r="D6" s="1" t="inlineStr">
@@ -546,7 +614,7 @@
       </c>
       <c r="C7" s="1" t="inlineStr">
         <is>
-          <t>8.6.1</t>
+          <t>8.7.0</t>
         </is>
       </c>
       <c r="D7" s="1" t="inlineStr">
@@ -610,7 +678,7 @@
       </c>
       <c r="C9" s="1" t="inlineStr">
         <is>
-          <t>99.4.501</t>
+          <t>101.4.434</t>
         </is>
       </c>
       <c r="D9" s="1" t="inlineStr">
@@ -738,7 +806,7 @@
       </c>
       <c r="C13" s="1" t="inlineStr">
         <is>
-          <t>12.00</t>
+          <t>12.01</t>
         </is>
       </c>
       <c r="D13" s="1" t="inlineStr">
@@ -802,7 +870,7 @@
       </c>
       <c r="C15" s="1" t="inlineStr">
         <is>
-          <t>77.0.1</t>
+          <t>78.0.2</t>
         </is>
       </c>
       <c r="D15" s="1" t="inlineStr">
@@ -930,7 +998,7 @@
       </c>
       <c r="C19" s="1" t="inlineStr">
         <is>
-          <t>6.26</t>
+          <t>6.28</t>
         </is>
       </c>
       <c r="D19" s="1" t="inlineStr">
@@ -994,7 +1062,7 @@
       </c>
       <c r="C21" s="1" t="inlineStr">
         <is>
-          <t>15.5.0</t>
+          <t>15.6.0</t>
         </is>
       </c>
       <c r="D21" s="1" t="inlineStr">
@@ -1026,7 +1094,7 @@
       </c>
       <c r="C22" s="1" t="inlineStr">
         <is>
-          <t>47.0.0</t>
+          <t>48.0.0</t>
         </is>
       </c>
       <c r="D22" s="1" t="inlineStr">
@@ -1218,7 +1286,7 @@
       </c>
       <c r="C28" s="1" t="inlineStr">
         <is>
-          <t>1.46</t>
+          <t>1.47</t>
         </is>
       </c>
       <c r="D28" s="1" t="inlineStr">
@@ -1272,27 +1340,27 @@
     <row r="30">
       <c r="A30" s="1" t="inlineStr">
         <is>
-          <t>g_play_music</t>
+          <t>yt_music</t>
         </is>
       </c>
       <c r="B30" s="1" t="inlineStr">
         <is>
-          <t>Google Play Music Desktop</t>
+          <t>YouTube Music</t>
         </is>
       </c>
       <c r="C30" s="1" t="inlineStr">
         <is>
-          <t>4.7.1</t>
+          <t>1.11.0</t>
         </is>
       </c>
       <c r="D30" s="1" t="inlineStr">
         <is>
-          <t>https://github.com/MarshallOfSound/Google-Play-Music-Desktop-Player-UNOFFICIAL-/releases</t>
+          <t>https://github.com/ytmdesktop/ytmdesktop/releases</t>
         </is>
       </c>
       <c r="E30" s="1" t="inlineStr">
         <is>
-          <t>https://github.com/MarshallOfSound/Google-Play-Music-Desktop-Player-UNOFFICIAL-/releases</t>
+          <t>https://github.com/ytmdesktop/ytmdesktop/releases</t>
         </is>
       </c>
       <c r="F30" t="inlineStr">
@@ -1314,7 +1382,7 @@
       </c>
       <c r="C31" s="1" t="inlineStr">
         <is>
-          <t>14.0.1</t>
+          <t>more</t>
         </is>
       </c>
       <c r="D31" s="1" t="inlineStr">

</xml_diff>

<commit_message>
App list updated with latest versions from the web
</commit_message>
<xml_diff>
--- a/apps_info.xlsx
+++ b/apps_info.xlsx
@@ -550,7 +550,7 @@
       </c>
       <c r="C5" s="1" t="inlineStr">
         <is>
-          <t>4.20.0</t>
+          <t>4.21.0</t>
         </is>
       </c>
       <c r="D5" s="1" t="inlineStr">
@@ -678,7 +678,7 @@
       </c>
       <c r="C9" s="1" t="inlineStr">
         <is>
-          <t>101.4.434</t>
+          <t>102.4.431</t>
         </is>
       </c>
       <c r="D9" s="1" t="inlineStr">
@@ -774,7 +774,7 @@
       </c>
       <c r="C12" s="1" t="inlineStr">
         <is>
-          <t>1.4.1.969</t>
+          <t>1.4.1.986</t>
         </is>
       </c>
       <c r="D12" s="1" t="inlineStr">
@@ -1190,7 +1190,7 @@
       </c>
       <c r="C25" s="1" t="inlineStr">
         <is>
-          <t>3.8.3</t>
+          <t>3.8.5</t>
         </is>
       </c>
       <c r="D25" s="1" t="inlineStr">
@@ -1350,7 +1350,7 @@
       </c>
       <c r="C30" s="1" t="inlineStr">
         <is>
-          <t>1.11.0</t>
+          <t>1.12.0-beta</t>
         </is>
       </c>
       <c r="D30" s="1" t="inlineStr">

</xml_diff>

<commit_message>
Add ffmpeg check from github page
</commit_message>
<xml_diff>
--- a/apps_info.xlsx
+++ b/apps_info.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <bookViews>
-    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="2985" yWindow="3180" windowWidth="21645" windowHeight="12525" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
+    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="-120" yWindow="480" windowWidth="29040" windowHeight="15840" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
     <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
@@ -391,10 +391,10 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F31"/>
+  <dimension ref="A1:F32"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
@@ -405,8 +405,8 @@
     <col width="47.140625" customWidth="1" style="1" min="4" max="4"/>
     <col width="88.7109375" bestFit="1" customWidth="1" style="1" min="5" max="5"/>
     <col width="55.85546875" customWidth="1" style="1" min="6" max="6"/>
-    <col width="9.140625" customWidth="1" style="1" min="7" max="15"/>
-    <col width="9.140625" customWidth="1" style="1" min="16" max="16384"/>
+    <col width="9.140625" customWidth="1" style="1" min="7" max="17"/>
+    <col width="9.140625" customWidth="1" style="1" min="18" max="16384"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -454,7 +454,7 @@
       </c>
       <c r="C2" s="1" t="inlineStr">
         <is>
-          <t>0.33.0</t>
+          <t>0.37.0</t>
         </is>
       </c>
       <c r="D2" s="1" t="inlineStr">
@@ -550,7 +550,7 @@
       </c>
       <c r="C5" s="1" t="inlineStr">
         <is>
-          <t>4.21.0</t>
+          <t>5.0.1</t>
         </is>
       </c>
       <c r="D5" s="1" t="inlineStr">
@@ -582,7 +582,7 @@
       </c>
       <c r="C6" s="1" t="inlineStr">
         <is>
-          <t>1.3.15 2020/06/26</t>
+          <t>1.3.16 2020/07/29</t>
         </is>
       </c>
       <c r="D6" s="1" t="inlineStr">
@@ -614,7 +614,7 @@
       </c>
       <c r="C7" s="1" t="inlineStr">
         <is>
-          <t>8.7.0</t>
+          <t>8.8.8</t>
         </is>
       </c>
       <c r="D7" s="1" t="inlineStr">
@@ -678,7 +678,7 @@
       </c>
       <c r="C9" s="1" t="inlineStr">
         <is>
-          <t>102.4.431</t>
+          <t>106.4.368</t>
         </is>
       </c>
       <c r="D9" s="1" t="inlineStr">
@@ -742,7 +742,7 @@
       </c>
       <c r="C11" s="1" t="inlineStr">
         <is>
-          <t>2020-03-08</t>
+          <t>2020-09-09</t>
         </is>
       </c>
       <c r="D11" s="1" t="inlineStr">
@@ -774,7 +774,7 @@
       </c>
       <c r="C12" s="1" t="inlineStr">
         <is>
-          <t>1.4.1.986</t>
+          <t>1.4.1.992</t>
         </is>
       </c>
       <c r="D12" s="1" t="inlineStr">
@@ -806,7 +806,7 @@
       </c>
       <c r="C13" s="1" t="inlineStr">
         <is>
-          <t>12.01</t>
+          <t>12.06</t>
         </is>
       </c>
       <c r="D13" s="1" t="inlineStr">
@@ -860,542 +860,574 @@
     <row r="15">
       <c r="A15" s="1" t="inlineStr">
         <is>
-          <t>firefox</t>
+          <t>ffmpeg</t>
         </is>
       </c>
       <c r="B15" s="1" t="inlineStr">
         <is>
-          <t>Firefox</t>
+          <t>FFmpeg</t>
         </is>
       </c>
       <c r="C15" s="1" t="inlineStr">
         <is>
-          <t>78.0.2</t>
+          <t>2020-09-27 12:31</t>
         </is>
       </c>
       <c r="D15" s="1" t="inlineStr">
         <is>
-          <t>https://en.wikipedia.org/wiki/Firefox</t>
+          <t>https://github.com/BtbN/FFmpeg-Builds/releases</t>
         </is>
       </c>
       <c r="E15" s="1" t="inlineStr">
         <is>
-          <t>https://download.mozilla.org/?product=firefox-latest-ssl^&amp;os=win64^&amp;lang=en-US</t>
+          <t>https://github.com/BtbN/FFmpeg-Builds/releases</t>
         </is>
       </c>
       <c r="F15" s="1" t="inlineStr">
         <is>
-          <t>//table[@class="infobox vevent"]/tbody/tr/td//text()</t>
+          <t>//div[@class="f1 flex-auto min-width-0 text-normal"]/a/text()</t>
         </is>
       </c>
     </row>
     <row r="16">
       <c r="A16" s="1" t="inlineStr">
         <is>
-          <t>git</t>
+          <t>firefox</t>
         </is>
       </c>
       <c r="B16" s="1" t="inlineStr">
         <is>
-          <t>Git</t>
+          <t>Firefox</t>
         </is>
       </c>
       <c r="C16" s="1" t="inlineStr">
         <is>
-          <t>2.27.0</t>
+          <t>81.0</t>
         </is>
       </c>
       <c r="D16" s="1" t="inlineStr">
         <is>
-          <t>https://git-scm.com/download/win</t>
+          <t>https://en.wikipedia.org/wiki/Firefox</t>
         </is>
       </c>
       <c r="E16" s="1" t="inlineStr">
         <is>
-          <t>https://git-scm.com/download/win</t>
+          <t>https://download.mozilla.org/?product=firefox-latest-ssl^&amp;os=win64^&amp;lang=en-US</t>
         </is>
       </c>
       <c r="F16" s="1" t="inlineStr">
         <is>
-          <t>//p[1]/strong[1]/text()</t>
+          <t>//table[@class="infobox vevent"]/tbody/tr/td//text()</t>
         </is>
       </c>
     </row>
     <row r="17">
       <c r="A17" s="1" t="inlineStr">
         <is>
-          <t>greenshot</t>
+          <t>git</t>
         </is>
       </c>
       <c r="B17" s="1" t="inlineStr">
         <is>
-          <t>Greenshot</t>
+          <t>Git</t>
         </is>
       </c>
       <c r="C17" s="1" t="inlineStr">
         <is>
-          <t>1.2.10.6</t>
+          <t>2.28.0</t>
         </is>
       </c>
       <c r="D17" s="1" t="inlineStr">
         <is>
-          <t>https://getgreenshot.org/downloads</t>
+          <t>https://git-scm.com/download/win</t>
         </is>
       </c>
       <c r="E17" s="1" t="inlineStr">
         <is>
-          <t>https://getgreenshot.org/downloads</t>
+          <t>https://git-scm.com/download/win</t>
         </is>
       </c>
       <c r="F17" s="1" t="inlineStr">
         <is>
-          <t>//div[2]/div[1]/div[1]/text()</t>
+          <t>//p[1]/strong[1]/text()</t>
         </is>
       </c>
     </row>
     <row r="18">
       <c r="A18" s="1" t="inlineStr">
         <is>
-          <t>hashtab</t>
+          <t>greenshot</t>
         </is>
       </c>
       <c r="B18" s="1" t="inlineStr">
         <is>
-          <t>Hashtab</t>
+          <t>Greenshot</t>
         </is>
       </c>
       <c r="C18" s="1" t="inlineStr">
         <is>
-          <t>6.0.0.34</t>
+          <t>1.2.10.6</t>
         </is>
       </c>
       <c r="D18" s="1" t="inlineStr">
         <is>
-          <t>http://implbits.com/products/hashtab</t>
+          <t>https://getgreenshot.org/downloads</t>
         </is>
       </c>
       <c r="E18" s="1" t="inlineStr">
         <is>
-          <t>http://implbits.com/products/hashtab</t>
+          <t>https://getgreenshot.org/downloads</t>
         </is>
       </c>
       <c r="F18" s="1" t="inlineStr">
         <is>
-          <t>//a[@id="btn_download_now"]</t>
+          <t>//div[2]/div[1]/div[1]/text()</t>
         </is>
       </c>
     </row>
     <row r="19">
       <c r="A19" s="1" t="inlineStr">
         <is>
-          <t>hwinfo</t>
+          <t>hashtab</t>
         </is>
       </c>
       <c r="B19" s="1" t="inlineStr">
         <is>
-          <t>HWInfo</t>
+          <t>Hashtab</t>
         </is>
       </c>
       <c r="C19" s="1" t="inlineStr">
         <is>
-          <t>6.28</t>
+          <t>6.0.0.34</t>
         </is>
       </c>
       <c r="D19" s="1" t="inlineStr">
         <is>
-          <t>https://www.hwinfo.com/download</t>
+          <t>http://implbits.com/products/hashtab</t>
         </is>
       </c>
       <c r="E19" s="1" t="inlineStr">
         <is>
-          <t>https://www.hwinfo.com/download</t>
+          <t>http://implbits.com/products/hashtab</t>
         </is>
       </c>
       <c r="F19" s="1" t="inlineStr">
         <is>
-          <t>//sub/text()</t>
+          <t>//a[@id="btn_download_now"]</t>
         </is>
       </c>
     </row>
     <row r="20">
       <c r="A20" s="1" t="inlineStr">
         <is>
-          <t>itunes</t>
+          <t>hwinfo</t>
         </is>
       </c>
       <c r="B20" s="1" t="inlineStr">
         <is>
-          <t>iTunes</t>
+          <t>HWInfo</t>
         </is>
       </c>
       <c r="C20" s="1" t="inlineStr">
         <is>
-          <t>12.10.7</t>
+          <t>6.30</t>
         </is>
       </c>
       <c r="D20" s="1" t="inlineStr">
         <is>
-          <t>https://en.wikipedia.org/wiki/ITunes</t>
+          <t>https://www.hwinfo.com/download</t>
         </is>
       </c>
       <c r="E20" s="1" t="inlineStr">
         <is>
-          <t>https://www.apple.com/itunes/download/win64</t>
+          <t>https://www.hwinfo.com/download</t>
         </is>
       </c>
       <c r="F20" s="1" t="inlineStr">
         <is>
-          <t>//table[@class="infobox vevent"]/tbody/tr/td//text()</t>
+          <t>//sub/text()</t>
         </is>
       </c>
     </row>
     <row r="21">
       <c r="A21" s="1" t="inlineStr">
         <is>
-          <t>klite_codec</t>
+          <t>itunes</t>
         </is>
       </c>
       <c r="B21" s="1" t="inlineStr">
         <is>
-          <t>K-Lite Codec</t>
+          <t>iTunes</t>
         </is>
       </c>
       <c r="C21" s="1" t="inlineStr">
         <is>
-          <t>15.6.0</t>
+          <t>12.10.9.3</t>
         </is>
       </c>
       <c r="D21" s="1" t="inlineStr">
         <is>
-          <t>https://codecguide.com/download_k-lite_codec_pack_standard.htm</t>
+          <t>https://en.wikipedia.org/wiki/ITunes</t>
         </is>
       </c>
       <c r="E21" s="1" t="inlineStr">
         <is>
-          <t>https://codecguide.com/download_k-lite_codec_pack_standard.htm</t>
+          <t>https://www.apple.com/itunes/download/win64</t>
         </is>
       </c>
       <c r="F21" s="1" t="inlineStr">
         <is>
-          <t>//h4/text()</t>
+          <t>//table[@class="infobox vevent"]/tbody/tr/td//text()</t>
         </is>
       </c>
     </row>
     <row r="22">
       <c r="A22" s="1" t="inlineStr">
         <is>
-          <t>mkvtoolnix</t>
+          <t>klite_codec</t>
         </is>
       </c>
       <c r="B22" s="1" t="inlineStr">
         <is>
-          <t>MKVToolnix</t>
+          <t>K-Lite Codec</t>
         </is>
       </c>
       <c r="C22" s="1" t="inlineStr">
         <is>
-          <t>48.0.0</t>
+          <t>15.7.0</t>
         </is>
       </c>
       <c r="D22" s="1" t="inlineStr">
         <is>
-          <t>https://www.fosshub.com/MKVToolNix.html</t>
+          <t>https://codecguide.com/download_k-lite_codec_pack_standard.htm</t>
         </is>
       </c>
       <c r="E22" s="1" t="inlineStr">
         <is>
-          <t>https://www.fosshub.com/MKVToolNix.html</t>
+          <t>https://codecguide.com/download_k-lite_codec_pack_standard.htm</t>
         </is>
       </c>
       <c r="F22" s="1" t="inlineStr">
         <is>
-          <t>//dd[@itemprop="softwareVersion"]/text()</t>
+          <t>//h4/text()</t>
         </is>
       </c>
     </row>
     <row r="23">
       <c r="A23" s="1" t="inlineStr">
         <is>
-          <t>obs</t>
+          <t>mkvtoolnix</t>
         </is>
       </c>
       <c r="B23" s="1" t="inlineStr">
         <is>
-          <t>OBS</t>
+          <t>MKVToolnix</t>
         </is>
       </c>
       <c r="C23" s="1" t="inlineStr">
         <is>
-          <t>25.0.8</t>
+          <t>50.0.0</t>
         </is>
       </c>
       <c r="D23" s="1" t="inlineStr">
         <is>
-          <t>https://obsproject.com/download</t>
+          <t>https://www.fosshub.com/MKVToolNix.html</t>
         </is>
       </c>
       <c r="E23" s="1" t="inlineStr">
         <is>
-          <t>https://obsproject.com/download</t>
+          <t>https://www.fosshub.com/MKVToolNix.html</t>
         </is>
       </c>
       <c r="F23" s="1" t="inlineStr">
         <is>
-          <t>//span[@class="dl_ver"]/text()</t>
+          <t>//dd[@itemprop="softwareVersion"]/text()</t>
         </is>
       </c>
     </row>
     <row r="24">
       <c r="A24" s="1" t="inlineStr">
         <is>
-          <t>open_shell</t>
+          <t>obs</t>
         </is>
       </c>
       <c r="B24" s="1" t="inlineStr">
         <is>
-          <t>Open Shell</t>
+          <t>OBS</t>
         </is>
       </c>
       <c r="C24" s="1" t="inlineStr">
         <is>
-          <t>4.4.142</t>
+          <t>25.0.8</t>
         </is>
       </c>
       <c r="D24" s="1" t="inlineStr">
         <is>
-          <t>https://github.com/Open-Shell/Open-Shell-Menu/releases</t>
+          <t>https://obsproject.com/download</t>
         </is>
       </c>
       <c r="E24" s="1" t="inlineStr">
         <is>
-          <t>https://github.com/Open-Shell/Open-Shell-Menu/releases</t>
+          <t>https://obsproject.com/download</t>
         </is>
       </c>
       <c r="F24" s="1" t="inlineStr">
         <is>
-          <t>//div[@class="f1 flex-auto min-width-0 text-normal"]/a/text()</t>
+          <t>//span[@class="dl_ver"]/text()</t>
         </is>
       </c>
     </row>
     <row r="25">
       <c r="A25" s="1" t="inlineStr">
         <is>
-          <t>python</t>
+          <t>open_shell</t>
         </is>
       </c>
       <c r="B25" s="1" t="inlineStr">
         <is>
-          <t>Python</t>
+          <t>Open Shell</t>
         </is>
       </c>
       <c r="C25" s="1" t="inlineStr">
         <is>
-          <t>3.8.5</t>
+          <t>4.4.152</t>
         </is>
       </c>
       <c r="D25" s="1" t="inlineStr">
         <is>
-          <t>https://www.python.org/downloads</t>
+          <t>https://github.com/Open-Shell/Open-Shell-Menu/releases</t>
         </is>
       </c>
       <c r="E25" s="1" t="inlineStr">
         <is>
-          <t>https://www.python.org/downloads</t>
+          <t>https://github.com/Open-Shell/Open-Shell-Menu/releases</t>
         </is>
       </c>
       <c r="F25" s="1" t="inlineStr">
         <is>
-          <t>//a[@class="button"]/text()</t>
+          <t>//div[@class="f1 flex-auto min-width-0 text-normal"]/a/text()</t>
         </is>
       </c>
     </row>
     <row r="26">
       <c r="A26" s="1" t="inlineStr">
         <is>
-          <t>rufus</t>
+          <t>python</t>
         </is>
       </c>
       <c r="B26" s="1" t="inlineStr">
         <is>
-          <t>Rufus</t>
+          <t>Python</t>
         </is>
       </c>
       <c r="C26" s="1" t="inlineStr">
         <is>
-          <t>3.11</t>
+          <t>3.8.5</t>
         </is>
       </c>
       <c r="D26" s="1" t="inlineStr">
         <is>
-          <t>https://github.com/pbatard/rufus/releases/latest</t>
+          <t>https://www.python.org/downloads</t>
         </is>
       </c>
       <c r="E26" s="1" t="inlineStr">
         <is>
-          <t>https://github.com/pbatard/rufus/releases/latest</t>
-        </is>
-      </c>
-      <c r="F26" t="inlineStr">
-        <is>
-          <t>//div[@class="f1 flex-auto min-width-0 text-normal"]/a/text()</t>
+          <t>https://www.python.org/downloads</t>
+        </is>
+      </c>
+      <c r="F26" s="1" t="inlineStr">
+        <is>
+          <t>//a[@class="button"]/text()</t>
         </is>
       </c>
     </row>
     <row r="27">
       <c r="A27" s="1" t="inlineStr">
         <is>
-          <t>sublime_text</t>
+          <t>rufus</t>
         </is>
       </c>
       <c r="B27" s="1" t="inlineStr">
         <is>
-          <t>Sublime Text</t>
+          <t>Rufus</t>
         </is>
       </c>
       <c r="C27" s="1" t="inlineStr">
         <is>
-          <t>3210</t>
+          <t>3.11</t>
         </is>
       </c>
       <c r="D27" s="1" t="inlineStr">
         <is>
-          <t>https://www.sublimetext.com/3dev</t>
+          <t>https://github.com/pbatard/rufus/releases/latest</t>
         </is>
       </c>
       <c r="E27" s="1" t="inlineStr">
         <is>
-          <t>https://www.sublimetext.com/3dev</t>
+          <t>https://github.com/pbatard/rufus/releases/latest</t>
         </is>
       </c>
       <c r="F27" t="inlineStr">
         <is>
-          <t>//p[@class="latest"]/text()</t>
+          <t>//div[@class="f1 flex-auto min-width-0 text-normal"]/a/text()</t>
         </is>
       </c>
     </row>
     <row r="28">
       <c r="A28" s="1" t="inlineStr">
         <is>
-          <t>visual_studio_code</t>
+          <t>spotify</t>
         </is>
       </c>
       <c r="B28" s="1" t="inlineStr">
         <is>
-          <t>Visual Studio Code</t>
+          <t>Spotify</t>
         </is>
       </c>
       <c r="C28" s="1" t="inlineStr">
         <is>
-          <t>1.47</t>
+          <t>1.142.622.0</t>
         </is>
       </c>
       <c r="D28" s="1" t="inlineStr">
         <is>
-          <t>https://code.visualstudio.com/updates</t>
+          <t>https://en.wikipedia.org/wiki/Spotify</t>
         </is>
       </c>
       <c r="E28" s="1" t="inlineStr">
         <is>
-          <t>https://code.visualstudio.com/updates</t>
-        </is>
-      </c>
-      <c r="F28" t="inlineStr">
-        <is>
-          <t>//div[@class="col-sm-9 col-md-8 body"]/h1/text()</t>
+          <t>http://download.spotify.com/SpotifyFullSetup.exe</t>
+        </is>
+      </c>
+      <c r="F28" s="1" t="inlineStr">
+        <is>
+          <t>//table[@class="infobox vevent"]/tbody/tr/td//text()</t>
         </is>
       </c>
     </row>
     <row r="29">
       <c r="A29" s="1" t="inlineStr">
         <is>
-          <t>winscp</t>
+          <t>sublime_text</t>
         </is>
       </c>
       <c r="B29" s="1" t="inlineStr">
         <is>
-          <t>WinSCP</t>
+          <t>Sublime Text</t>
         </is>
       </c>
       <c r="C29" s="1" t="inlineStr">
         <is>
-          <t>5.17.6</t>
+          <t>3210</t>
         </is>
       </c>
       <c r="D29" s="1" t="inlineStr">
         <is>
-          <t>https://winscp.net/eng/download.php</t>
+          <t>https://www.sublimetext.com/3dev</t>
         </is>
       </c>
       <c r="E29" s="1" t="inlineStr">
         <is>
-          <t>https://winscp.net/eng/download.php</t>
+          <t>https://www.sublimetext.com/3dev</t>
         </is>
       </c>
       <c r="F29" t="inlineStr">
         <is>
-          <t>//a[@class="btn btn-primary btn-lg"]/text()</t>
+          <t>//p[@class="latest"]/text()</t>
         </is>
       </c>
     </row>
     <row r="30">
       <c r="A30" s="1" t="inlineStr">
         <is>
-          <t>yt_music</t>
+          <t>visual_studio_code</t>
         </is>
       </c>
       <c r="B30" s="1" t="inlineStr">
         <is>
-          <t>YouTube Music</t>
+          <t>Visual Studio Code</t>
         </is>
       </c>
       <c r="C30" s="1" t="inlineStr">
         <is>
-          <t>1.12.0-beta</t>
+          <t>1.49</t>
         </is>
       </c>
       <c r="D30" s="1" t="inlineStr">
         <is>
-          <t>https://github.com/ytmdesktop/ytmdesktop/releases</t>
+          <t>https://code.visualstudio.com/updates</t>
         </is>
       </c>
       <c r="E30" s="1" t="inlineStr">
         <is>
-          <t>https://github.com/ytmdesktop/ytmdesktop/releases</t>
+          <t>https://code.visualstudio.com/updates</t>
         </is>
       </c>
       <c r="F30" t="inlineStr">
         <is>
-          <t>//div[@class="f1 flex-auto min-width-0 text-normal"]/a/text()</t>
+          <t>//div[@class="col-sm-9 col-md-8 body"]/h1/text()</t>
         </is>
       </c>
     </row>
     <row r="31">
       <c r="A31" s="1" t="inlineStr">
         <is>
+          <t>winscp</t>
+        </is>
+      </c>
+      <c r="B31" s="1" t="inlineStr">
+        <is>
+          <t>WinSCP</t>
+        </is>
+      </c>
+      <c r="C31" s="1" t="inlineStr">
+        <is>
+          <t>5.17.7</t>
+        </is>
+      </c>
+      <c r="D31" s="1" t="inlineStr">
+        <is>
+          <t>https://winscp.net/eng/download.php</t>
+        </is>
+      </c>
+      <c r="E31" s="1" t="inlineStr">
+        <is>
+          <t>https://winscp.net/eng/download.php</t>
+        </is>
+      </c>
+      <c r="F31" t="inlineStr">
+        <is>
+          <t>//a[@class="btn btn-primary btn-lg"]/text()</t>
+        </is>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" s="1" t="inlineStr">
+        <is>
           <t>java</t>
         </is>
       </c>
-      <c r="B31" s="1" t="inlineStr">
+      <c r="B32" s="1" t="inlineStr">
         <is>
           <t>Java SE</t>
         </is>
       </c>
-      <c r="C31" s="1" t="inlineStr">
-        <is>
-          <t>more</t>
-        </is>
-      </c>
-      <c r="D31" s="1" t="inlineStr">
+      <c r="C32" s="1" t="inlineStr">
+        <is>
+          <t>15</t>
+        </is>
+      </c>
+      <c r="D32" s="1" t="inlineStr">
         <is>
           <t>https://www.oracle.com/java/technologies/javase-downloads.html</t>
         </is>
       </c>
-      <c r="E31" s="1" t="inlineStr">
+      <c r="E32" s="1" t="inlineStr">
         <is>
           <t>https://www.oracle.com/java/technologies/javase-downloads.html</t>
         </is>
       </c>
-      <c r="F31" s="1" t="inlineStr">
+      <c r="F32" s="1" t="inlineStr">
         <is>
           <t>//p/text()</t>
         </is>

</xml_diff>

<commit_message>
Update excel file with latest versions
</commit_message>
<xml_diff>
--- a/apps_info.xlsx
+++ b/apps_info.xlsx
@@ -454,7 +454,7 @@
       </c>
       <c r="C2" s="1" t="inlineStr">
         <is>
-          <t>0.37.0</t>
+          <t>0.39.0</t>
         </is>
       </c>
       <c r="D2" s="1" t="inlineStr">
@@ -550,7 +550,7 @@
       </c>
       <c r="C5" s="1" t="inlineStr">
         <is>
-          <t>5.0.1</t>
+          <t>5.5.0</t>
         </is>
       </c>
       <c r="D5" s="1" t="inlineStr">
@@ -614,7 +614,7 @@
       </c>
       <c r="C7" s="1" t="inlineStr">
         <is>
-          <t>8.8.8</t>
+          <t>8.8.9</t>
         </is>
       </c>
       <c r="D7" s="1" t="inlineStr">
@@ -646,7 +646,7 @@
       </c>
       <c r="C8" s="1" t="inlineStr">
         <is>
-          <t>7.0.0h</t>
+          <t>8.0.0</t>
         </is>
       </c>
       <c r="D8" s="1" t="inlineStr">
@@ -678,7 +678,7 @@
       </c>
       <c r="C9" s="1" t="inlineStr">
         <is>
-          <t>106.4.368</t>
+          <t>110.4.458</t>
         </is>
       </c>
       <c r="D9" s="1" t="inlineStr">
@@ -806,7 +806,7 @@
       </c>
       <c r="C13" s="1" t="inlineStr">
         <is>
-          <t>12.06</t>
+          <t>12.10</t>
         </is>
       </c>
       <c r="D13" s="1" t="inlineStr">
@@ -870,7 +870,7 @@
       </c>
       <c r="C15" s="1" t="inlineStr">
         <is>
-          <t>2020-09-27 12:31</t>
+          <t>2020-11-20 12:39</t>
         </is>
       </c>
       <c r="D15" s="1" t="inlineStr">
@@ -902,7 +902,7 @@
       </c>
       <c r="C16" s="1" t="inlineStr">
         <is>
-          <t>81.0</t>
+          <t>83.0</t>
         </is>
       </c>
       <c r="D16" s="1" t="inlineStr">
@@ -934,7 +934,7 @@
       </c>
       <c r="C17" s="1" t="inlineStr">
         <is>
-          <t>2.28.0</t>
+          <t>2.29.2</t>
         </is>
       </c>
       <c r="D17" s="1" t="inlineStr">
@@ -1030,7 +1030,7 @@
       </c>
       <c r="C20" s="1" t="inlineStr">
         <is>
-          <t>6.30</t>
+          <t>6.34</t>
         </is>
       </c>
       <c r="D20" s="1" t="inlineStr">
@@ -1062,7 +1062,7 @@
       </c>
       <c r="C21" s="1" t="inlineStr">
         <is>
-          <t>12.10.9.3</t>
+          <t>12.11.0.26</t>
         </is>
       </c>
       <c r="D21" s="1" t="inlineStr">
@@ -1094,7 +1094,7 @@
       </c>
       <c r="C22" s="1" t="inlineStr">
         <is>
-          <t>15.7.0</t>
+          <t>15.8.7</t>
         </is>
       </c>
       <c r="D22" s="1" t="inlineStr">
@@ -1126,7 +1126,7 @@
       </c>
       <c r="C23" s="1" t="inlineStr">
         <is>
-          <t>50.0.0</t>
+          <t>51.0.0</t>
         </is>
       </c>
       <c r="D23" s="1" t="inlineStr">
@@ -1158,7 +1158,7 @@
       </c>
       <c r="C24" s="1" t="inlineStr">
         <is>
-          <t>25.0.8</t>
+          <t>26.0.2</t>
         </is>
       </c>
       <c r="D24" s="1" t="inlineStr">
@@ -1190,7 +1190,7 @@
       </c>
       <c r="C25" s="1" t="inlineStr">
         <is>
-          <t>4.4.152</t>
+          <t>4.4.160</t>
         </is>
       </c>
       <c r="D25" s="1" t="inlineStr">
@@ -1222,7 +1222,7 @@
       </c>
       <c r="C26" s="1" t="inlineStr">
         <is>
-          <t>3.8.5</t>
+          <t>3.9.0</t>
         </is>
       </c>
       <c r="D26" s="1" t="inlineStr">
@@ -1254,7 +1254,7 @@
       </c>
       <c r="C27" s="1" t="inlineStr">
         <is>
-          <t>3.11</t>
+          <t>3.13</t>
         </is>
       </c>
       <c r="D27" s="1" t="inlineStr">
@@ -1286,7 +1286,7 @@
       </c>
       <c r="C28" s="1" t="inlineStr">
         <is>
-          <t>1.142.622.0</t>
+          <t>1.146.916.0</t>
         </is>
       </c>
       <c r="D28" s="1" t="inlineStr">
@@ -1350,7 +1350,7 @@
       </c>
       <c r="C30" s="1" t="inlineStr">
         <is>
-          <t>1.49</t>
+          <t>1.51</t>
         </is>
       </c>
       <c r="D30" s="1" t="inlineStr">
@@ -1382,7 +1382,7 @@
       </c>
       <c r="C31" s="1" t="inlineStr">
         <is>
-          <t>5.17.7</t>
+          <t>5.17.9</t>
         </is>
       </c>
       <c r="D31" s="1" t="inlineStr">
@@ -1414,7 +1414,7 @@
       </c>
       <c r="C32" s="1" t="inlineStr">
         <is>
-          <t>15</t>
+          <t>15.0.1</t>
         </is>
       </c>
       <c r="D32" s="1" t="inlineStr">

</xml_diff>